<commit_message>
se agrego funcion a 2FN y coreccion de las llaves en lectura de archivo
</commit_message>
<xml_diff>
--- a/formato.xlsx
+++ b/formato.xlsx
@@ -509,9 +509,9 @@
 <office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.3">
   <office:meta>
     <meta:creation-date>2024-08-06T13:16:12.509276145</meta:creation-date>
-    <dc:date>2024-08-13T06:55:00.975420597</dc:date>
-    <meta:editing-duration>PT5H17M56S</meta:editing-duration>
-    <meta:editing-cycles>21</meta:editing-cycles>
+    <dc:date>2024-08-13T08:14:02.395698059</dc:date>
+    <meta:editing-duration>PT6H13M16S</meta:editing-duration>
+    <meta:editing-cycles>22</meta:editing-cycles>
     <meta:generator>LibreOffice/24.2.5.2$Linux_X86_64 LibreOffice_project/420$Build-2</meta:generator>
     <meta:document-statistic meta:table-count="2" meta:cell-count="112" meta:object-count="0"/>
   </office:meta>
@@ -531,8 +531,8 @@
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
-              <config:config-item config:name="CursorPositionX" config:type="int">5</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">11</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">6</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>

</xml_diff>